<commit_message>
fix thừa thông tin thiết kế newfeeds
</commit_message>
<xml_diff>
--- a/documents/Front-end Design.xlsx
+++ b/documents/Front-end Design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Landing page" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
   <si>
     <t>Nội dung trang</t>
   </si>
@@ -759,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -1293,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,7 +1314,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1322,38 +1322,6 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>